<commit_message>
adapted the code to handle experimental data collected on 230718
</commit_message>
<xml_diff>
--- a/indentation/experiments/texturometer/processed_data/texturometer_forces.xlsx
+++ b/indentation/experiments/texturometer/processed_data/texturometer_forces.xlsx
@@ -1,31 +1,42 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\siaquinta\Documents\Projet Périnée\perineal_indentation\indentation\experiments\texturometer\processed_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C54DB66-6C25-428F-8436-0CE9616E2772}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BE63FEC-D4D5-49D8-9E11-3AD6AF5E1DD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-5670" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="428" uniqueCount="428">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="500" uniqueCount="500">
   <si>
     <t>Id</t>
   </si>
@@ -1309,6 +1320,222 @@
   </si>
   <si>
     <t>F80</t>
+  </si>
+  <si>
+    <t>230718_FF1_A</t>
+  </si>
+  <si>
+    <t>230718_FF1_B</t>
+  </si>
+  <si>
+    <t>230718_FF1_C</t>
+  </si>
+  <si>
+    <t>230718_FF2_A</t>
+  </si>
+  <si>
+    <t>230718_FF2_B</t>
+  </si>
+  <si>
+    <t>230718_FF2_C</t>
+  </si>
+  <si>
+    <t>230718_FF3_A</t>
+  </si>
+  <si>
+    <t>230718_FF3_B</t>
+  </si>
+  <si>
+    <t>230718_FF3_C</t>
+  </si>
+  <si>
+    <t>230718_FF4_A</t>
+  </si>
+  <si>
+    <t>230718_FF4_B</t>
+  </si>
+  <si>
+    <t>230718_FF4_C</t>
+  </si>
+  <si>
+    <t>230718_FF5_A</t>
+  </si>
+  <si>
+    <t>230718_FF5_B</t>
+  </si>
+  <si>
+    <t>230718_FF5_C</t>
+  </si>
+  <si>
+    <t>230718_FF1_D</t>
+  </si>
+  <si>
+    <t>230718_FF1_E</t>
+  </si>
+  <si>
+    <t>230718_FF2_D</t>
+  </si>
+  <si>
+    <t>230718_FF2_E</t>
+  </si>
+  <si>
+    <t>230718_FF3_D</t>
+  </si>
+  <si>
+    <t>230718_FF4_D</t>
+  </si>
+  <si>
+    <t>230718_FF5_D</t>
+  </si>
+  <si>
+    <t>230718_FF5_E</t>
+  </si>
+  <si>
+    <t>230718_FF5_F</t>
+  </si>
+  <si>
+    <t>4.06632804870642</t>
+  </si>
+  <si>
+    <t>97.6550598144529</t>
+  </si>
+  <si>
+    <t>16.2561569213866</t>
+  </si>
+  <si>
+    <t>50.7060813903802</t>
+  </si>
+  <si>
+    <t>15.254155158996</t>
+  </si>
+  <si>
+    <t>28.4071407318117</t>
+  </si>
+  <si>
+    <t>7.65582656860374</t>
+  </si>
+  <si>
+    <t>53.2443695068363</t>
+  </si>
+  <si>
+    <t>19.1822929382315</t>
+  </si>
+  <si>
+    <t>61.8381805419913</t>
+  </si>
+  <si>
+    <t>8.89438629150381</t>
+  </si>
+  <si>
+    <t>45.6641693115232</t>
+  </si>
+  <si>
+    <t>4.27507400512669</t>
+  </si>
+  <si>
+    <t>47.7472496032698</t>
+  </si>
+  <si>
+    <t>19.6130981445324</t>
+  </si>
+  <si>
+    <t>49.5825653076173</t>
+  </si>
+  <si>
+    <t>7.58116197585891</t>
+  </si>
+  <si>
+    <t>48.5847244262693</t>
+  </si>
+  <si>
+    <t>20.1609725952161</t>
+  </si>
+  <si>
+    <t>74.8009185791046</t>
+  </si>
+  <si>
+    <t>4.770984172821</t>
+  </si>
+  <si>
+    <t>72.1743392944364</t>
+  </si>
+  <si>
+    <t>9.43238544464287</t>
+  </si>
+  <si>
+    <t>55.0407867431644</t>
+  </si>
+  <si>
+    <t>11.138648033142</t>
+  </si>
+  <si>
+    <t>101.482803344719</t>
+  </si>
+  <si>
+    <t>26.9608497619636</t>
+  </si>
+  <si>
+    <t>67.6510696411109</t>
+  </si>
+  <si>
+    <t>13.2886114120482</t>
+  </si>
+  <si>
+    <t>81.6852111816406</t>
+  </si>
+  <si>
+    <t>14.3018760681141</t>
+  </si>
+  <si>
+    <t>49.6651878356928</t>
+  </si>
+  <si>
+    <t>2.9882698059083</t>
+  </si>
+  <si>
+    <t>24.8318862915028</t>
+  </si>
+  <si>
+    <t>14.8666410446173</t>
+  </si>
+  <si>
+    <t>33.0632324218743</t>
+  </si>
+  <si>
+    <t>16.0089015960688</t>
+  </si>
+  <si>
+    <t>43.2277221679739</t>
+  </si>
+  <si>
+    <t>25.1563796997044</t>
+  </si>
+  <si>
+    <t>48.6795845031718</t>
+  </si>
+  <si>
+    <t>10.8912563323974</t>
+  </si>
+  <si>
+    <t>27.513494491578</t>
+  </si>
+  <si>
+    <t>6.42561435699454</t>
+  </si>
+  <si>
+    <t>45.5603981018074</t>
+  </si>
+  <si>
+    <t>16.1440563201911</t>
+  </si>
+  <si>
+    <t>47.3149795532241</t>
+  </si>
+  <si>
+    <t>11.783949851989</t>
+  </si>
+  <si>
+    <t>30.7021770477293</t>
   </si>
 </sst>
 </file>
@@ -1626,13 +1853,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E142"/>
+  <dimension ref="A1:E166"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+    <sheetView tabSelected="1" topLeftCell="A146" workbookViewId="0">
+      <selection activeCell="G163" sqref="G163"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.7109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -4045,6 +4275,414 @@
         <v>425</v>
       </c>
       <c r="E142">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A143" t="s">
+        <v>428</v>
+      </c>
+      <c r="B143">
+        <v>230718</v>
+      </c>
+      <c r="C143" t="s">
+        <v>452</v>
+      </c>
+      <c r="D143" t="s">
+        <v>453</v>
+      </c>
+      <c r="E143">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A144" t="s">
+        <v>429</v>
+      </c>
+      <c r="B144">
+        <v>230718</v>
+      </c>
+      <c r="C144" t="s">
+        <v>454</v>
+      </c>
+      <c r="D144" t="s">
+        <v>455</v>
+      </c>
+      <c r="E144">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A145" t="s">
+        <v>430</v>
+      </c>
+      <c r="B145">
+        <v>230718</v>
+      </c>
+      <c r="C145" t="s">
+        <v>456</v>
+      </c>
+      <c r="D145" t="s">
+        <v>457</v>
+      </c>
+      <c r="E145">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A146" t="s">
+        <v>443</v>
+      </c>
+      <c r="B146">
+        <v>230718</v>
+      </c>
+      <c r="C146" t="s">
+        <v>458</v>
+      </c>
+      <c r="D146" t="s">
+        <v>459</v>
+      </c>
+      <c r="E146">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A147" t="s">
+        <v>444</v>
+      </c>
+      <c r="B147">
+        <v>230718</v>
+      </c>
+      <c r="C147" t="s">
+        <v>460</v>
+      </c>
+      <c r="D147" t="s">
+        <v>461</v>
+      </c>
+      <c r="E147">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A148" t="s">
+        <v>431</v>
+      </c>
+      <c r="B148">
+        <v>230718</v>
+      </c>
+      <c r="C148" t="s">
+        <v>462</v>
+      </c>
+      <c r="D148" t="s">
+        <v>463</v>
+      </c>
+      <c r="E148">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A149" t="s">
+        <v>432</v>
+      </c>
+      <c r="B149">
+        <v>230718</v>
+      </c>
+      <c r="C149" t="s">
+        <v>464</v>
+      </c>
+      <c r="D149" t="s">
+        <v>465</v>
+      </c>
+      <c r="E149">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A150" t="s">
+        <v>433</v>
+      </c>
+      <c r="B150">
+        <v>230718</v>
+      </c>
+      <c r="C150" t="s">
+        <v>466</v>
+      </c>
+      <c r="D150" t="s">
+        <v>467</v>
+      </c>
+      <c r="E150">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A151" t="s">
+        <v>445</v>
+      </c>
+      <c r="B151">
+        <v>230718</v>
+      </c>
+      <c r="C151" t="s">
+        <v>468</v>
+      </c>
+      <c r="D151" t="s">
+        <v>469</v>
+      </c>
+      <c r="E151">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A152" t="s">
+        <v>446</v>
+      </c>
+      <c r="B152">
+        <v>230718</v>
+      </c>
+      <c r="C152" t="s">
+        <v>470</v>
+      </c>
+      <c r="D152" t="s">
+        <v>471</v>
+      </c>
+      <c r="E152">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A153" t="s">
+        <v>434</v>
+      </c>
+      <c r="B153">
+        <v>230718</v>
+      </c>
+      <c r="C153" t="s">
+        <v>472</v>
+      </c>
+      <c r="D153" t="s">
+        <v>473</v>
+      </c>
+      <c r="E153">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A154" t="s">
+        <v>435</v>
+      </c>
+      <c r="B154">
+        <v>230718</v>
+      </c>
+      <c r="C154" t="s">
+        <v>474</v>
+      </c>
+      <c r="D154" t="s">
+        <v>475</v>
+      </c>
+      <c r="E154">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A155" t="s">
+        <v>436</v>
+      </c>
+      <c r="B155">
+        <v>230718</v>
+      </c>
+      <c r="C155" t="s">
+        <v>476</v>
+      </c>
+      <c r="D155" t="s">
+        <v>477</v>
+      </c>
+      <c r="E155">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A156" t="s">
+        <v>447</v>
+      </c>
+      <c r="B156">
+        <v>230718</v>
+      </c>
+      <c r="C156" t="s">
+        <v>478</v>
+      </c>
+      <c r="D156" t="s">
+        <v>479</v>
+      </c>
+      <c r="E156">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A157" t="s">
+        <v>437</v>
+      </c>
+      <c r="B157">
+        <v>230718</v>
+      </c>
+      <c r="C157" t="s">
+        <v>480</v>
+      </c>
+      <c r="D157" t="s">
+        <v>481</v>
+      </c>
+      <c r="E157">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A158" t="s">
+        <v>438</v>
+      </c>
+      <c r="B158">
+        <v>230718</v>
+      </c>
+      <c r="C158" t="s">
+        <v>482</v>
+      </c>
+      <c r="D158" t="s">
+        <v>483</v>
+      </c>
+      <c r="E158">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="159" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A159" t="s">
+        <v>439</v>
+      </c>
+      <c r="B159">
+        <v>230718</v>
+      </c>
+      <c r="C159" t="s">
+        <v>484</v>
+      </c>
+      <c r="D159" t="s">
+        <v>485</v>
+      </c>
+      <c r="E159">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A160" t="s">
+        <v>448</v>
+      </c>
+      <c r="B160">
+        <v>230718</v>
+      </c>
+      <c r="C160" t="s">
+        <v>486</v>
+      </c>
+      <c r="D160" t="s">
+        <v>487</v>
+      </c>
+      <c r="E160">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A161" t="s">
+        <v>440</v>
+      </c>
+      <c r="B161">
+        <v>230718</v>
+      </c>
+      <c r="C161" t="s">
+        <v>488</v>
+      </c>
+      <c r="D161" t="s">
+        <v>489</v>
+      </c>
+      <c r="E161">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A162" t="s">
+        <v>441</v>
+      </c>
+      <c r="B162">
+        <v>230718</v>
+      </c>
+      <c r="C162" t="s">
+        <v>490</v>
+      </c>
+      <c r="D162" t="s">
+        <v>491</v>
+      </c>
+      <c r="E162">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A163" t="s">
+        <v>442</v>
+      </c>
+      <c r="B163">
+        <v>230718</v>
+      </c>
+      <c r="C163" t="s">
+        <v>492</v>
+      </c>
+      <c r="D163" t="s">
+        <v>493</v>
+      </c>
+      <c r="E163">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="164" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A164" t="s">
+        <v>449</v>
+      </c>
+      <c r="B164">
+        <v>230718</v>
+      </c>
+      <c r="C164" t="s">
+        <v>494</v>
+      </c>
+      <c r="D164" t="s">
+        <v>495</v>
+      </c>
+      <c r="E164">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A165" t="s">
+        <v>450</v>
+      </c>
+      <c r="B165">
+        <v>230718</v>
+      </c>
+      <c r="C165" t="s">
+        <v>496</v>
+      </c>
+      <c r="D165" t="s">
+        <v>497</v>
+      </c>
+      <c r="E165">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A166" t="s">
+        <v>451</v>
+      </c>
+      <c r="B166">
+        <v>230718</v>
+      </c>
+      <c r="C166" t="s">
+        <v>498</v>
+      </c>
+      <c r="D166" t="s">
+        <v>499</v>
+      </c>
+      <c r="E166">
         <v>0</v>
       </c>
     </row>

</xml_diff>